<commit_message>
First Raw Data Batch
Added the first batch of raw data.
</commit_message>
<xml_diff>
--- a/Analysis/_TEMPLATE-ISSUES.xlsx
+++ b/Analysis/_TEMPLATE-ISSUES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Git Repositories\Good-First-Issue\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Git Repositories\Good-First-Issue\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383E144D-43BE-4B0A-A1BE-FEAB9A8EF6F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1647C625-F94C-4EE3-9F4A-9EFABFA5B527}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26295" yWindow="5850" windowWidth="38700" windowHeight="15435" xr2:uid="{BE161B33-A94A-4E68-B9E5-07DB50A2B4FE}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="38700" windowHeight="15435" xr2:uid="{BE161B33-A94A-4E68-B9E5-07DB50A2B4FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Issue</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Other Type</t>
+  </si>
+  <si>
+    <t>Refactoring(0/1)</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62907D4F-821C-42A5-BB97-2A16C8296F6E}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +447,7 @@
     <col min="13" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,9 +482,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>